<commit_message>
fixed bug with collision group mask
</commit_message>
<xml_diff>
--- a/ffxiv_mmd_tools_helper/data/rigid_body.xlsx
+++ b/ffxiv_mmd_tools_helper/data/rigid_body.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MMD\ffxiv_mmd_tools_helper\ffxiv_mmd_tools_helper_beta\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MMD\ffxiv_mmd_tools_helper\ffxiv_mmd_tools_helper\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4005AB4-099E-454B-9ED2-5FA9155A047E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B6CE3D-F19A-4A7F-9FD0-2ED6D4B31EA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43320" yWindow="1440" windowWidth="28800" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="1695" windowWidth="20820" windowHeight="14715" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="115">
   <si>
     <t>bone_name</t>
   </si>
@@ -365,6 +365,12 @@
   </si>
   <si>
     <t>j_sk_s_c_r</t>
+  </si>
+  <si>
+    <t>1/3/10</t>
+  </si>
+  <si>
+    <t>0/1</t>
   </si>
 </sst>
 </file>
@@ -500,7 +506,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -514,19 +520,20 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -550,13 +557,6 @@
           <bgColor theme="4"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-      </border>
     </dxf>
     <dxf>
       <border outline="0">
@@ -646,7 +646,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65851253-A80B-4DD0-9F1A-C557CFC2122C}" name="Table1" displayName="Table1" ref="A1:AI60" totalsRowShown="0" headerRowDxfId="0" tableBorderDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{65851253-A80B-4DD0-9F1A-C557CFC2122C}" name="Table1" displayName="Table1" ref="A1:AI60" totalsRowShown="0" headerRowDxfId="1" tableBorderDxfId="0">
   <autoFilter ref="A1:AI60" xr:uid="{65851253-A80B-4DD0-9F1A-C557CFC2122C}"/>
   <tableColumns count="35">
     <tableColumn id="1" xr3:uid="{6A8B691E-AF96-403F-B914-BFE48986FDFE}" name="rigid_body_name"/>
@@ -2369,8 +2369,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D213BE9-EC88-43A5-B10E-7AC8A26A2FF6}">
   <dimension ref="A1:AI60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y28" workbookViewId="0">
-      <selection activeCell="AD43" sqref="AD43"/>
+    <sheetView tabSelected="1" topLeftCell="R34" workbookViewId="0">
+      <selection activeCell="AA9" sqref="AA2:AA9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2414,103 +2414,103 @@
       <c r="A1" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="20" t="s">
+      <c r="B1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="10" t="s">
         <v>69</v>
       </c>
       <c r="F1" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="20" t="s">
+      <c r="K1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="20" t="s">
+      <c r="L1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="20" t="s">
+      <c r="M1" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="N1" s="20" t="s">
+      <c r="N1" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="O1" s="20" t="s">
+      <c r="O1" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="P1" s="20" t="s">
+      <c r="P1" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="Q1" s="20" t="s">
+      <c r="Q1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="R1" s="20" t="s">
+      <c r="R1" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="S1" s="20" t="s">
+      <c r="S1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="T1" s="20" t="s">
+      <c r="T1" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="U1" s="20" t="s">
+      <c r="U1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="V1" s="20" t="s">
+      <c r="V1" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="W1" s="20" t="s">
+      <c r="W1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="X1" s="20" t="s">
+      <c r="X1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="Y1" s="20" t="s">
+      <c r="Y1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="Z1" s="20" t="s">
+      <c r="Z1" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="AA1" s="20" t="s">
+      <c r="AA1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="AB1" s="20" t="s">
+      <c r="AB1" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="AC1" s="20" t="s">
+      <c r="AC1" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="AD1" s="20" t="s">
+      <c r="AD1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="AE1" s="20" t="s">
+      <c r="AE1" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="AF1" s="20" t="s">
+      <c r="AF1" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="AG1" s="20" t="s">
+      <c r="AG1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="AH1" s="20" t="s">
+      <c r="AH1" s="10" t="s">
         <v>26</v>
       </c>
       <c r="AI1" s="11" t="s">
@@ -2518,2470 +2518,2470 @@
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13">
+      <c r="A2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6">
         <v>0.06</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="6">
         <v>0.06</v>
       </c>
-      <c r="F2" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="13">
-        <v>0</v>
-      </c>
-      <c r="I2" s="13" t="s">
+      <c r="F2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="6">
+        <v>0</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="J2" s="13">
+      <c r="J2" s="6">
         <v>0.08</v>
       </c>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13">
-        <v>1</v>
-      </c>
-      <c r="T2" s="13"/>
-      <c r="U2" s="13"/>
-      <c r="V2" s="13">
-        <v>0</v>
-      </c>
-      <c r="W2" s="13">
-        <v>0</v>
-      </c>
-      <c r="X2" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="Y2" s="13"/>
-      <c r="Z2" s="13"/>
-      <c r="AA2" s="13">
-        <v>0</v>
-      </c>
-      <c r="AB2" s="13"/>
-      <c r="AC2" s="13"/>
-      <c r="AD2" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AE2" s="13"/>
-      <c r="AF2" s="13"/>
-      <c r="AG2" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AH2" s="13"/>
-      <c r="AI2" s="17"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6">
+        <v>1</v>
+      </c>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6">
+        <v>0</v>
+      </c>
+      <c r="W2" s="6">
+        <v>1</v>
+      </c>
+      <c r="X2" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6"/>
+      <c r="AA2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB2" s="6"/>
+      <c r="AC2" s="6"/>
+      <c r="AD2" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AE2" s="6"/>
+      <c r="AF2" s="6"/>
+      <c r="AG2" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AH2" s="6"/>
+      <c r="AI2" s="7"/>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="14" t="s">
+      <c r="B3" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="H3" s="13">
-        <v>0</v>
-      </c>
-      <c r="I3" s="13" t="s">
+      <c r="H3" s="6">
+        <v>0</v>
+      </c>
+      <c r="I3" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="J3" s="13">
+      <c r="J3" s="6">
         <v>0.05</v>
       </c>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="13">
-        <v>1</v>
-      </c>
-      <c r="T3" s="13"/>
-      <c r="U3" s="13"/>
-      <c r="V3" s="13">
-        <v>0</v>
-      </c>
-      <c r="W3" s="13">
-        <v>0</v>
-      </c>
-      <c r="X3" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="Y3" s="13"/>
-      <c r="Z3" s="13"/>
-      <c r="AA3" s="13">
-        <v>0</v>
-      </c>
-      <c r="AB3" s="13"/>
-      <c r="AC3" s="13"/>
-      <c r="AD3" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AE3" s="13"/>
-      <c r="AF3" s="13"/>
-      <c r="AG3" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AH3" s="13"/>
-      <c r="AI3" s="17"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="6"/>
+      <c r="S3" s="6">
+        <v>1</v>
+      </c>
+      <c r="T3" s="6"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6">
+        <v>0</v>
+      </c>
+      <c r="W3" s="6">
+        <v>1</v>
+      </c>
+      <c r="X3" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="Y3" s="6"/>
+      <c r="Z3" s="6"/>
+      <c r="AA3" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB3" s="6"/>
+      <c r="AC3" s="6"/>
+      <c r="AD3" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AE3" s="6"/>
+      <c r="AF3" s="6"/>
+      <c r="AG3" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AH3" s="6"/>
+      <c r="AI3" s="7"/>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="13">
-        <v>0</v>
-      </c>
-      <c r="I4" s="13" t="s">
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="6">
+        <v>0</v>
+      </c>
+      <c r="I4" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J4" s="13">
+      <c r="J4" s="6">
         <v>0.06</v>
       </c>
-      <c r="K4" s="13">
+      <c r="K4" s="6">
         <v>0.12</v>
       </c>
-      <c r="L4" s="13"/>
-      <c r="M4" s="13"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="13"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="13"/>
-      <c r="S4" s="13">
-        <v>1</v>
-      </c>
-      <c r="T4" s="13"/>
-      <c r="U4" s="13"/>
-      <c r="V4" s="13">
-        <v>0</v>
-      </c>
-      <c r="W4" s="13">
-        <v>0</v>
-      </c>
-      <c r="X4" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="Y4" s="13"/>
-      <c r="Z4" s="13"/>
-      <c r="AA4" s="13">
-        <v>0</v>
-      </c>
-      <c r="AB4" s="13"/>
-      <c r="AC4" s="13"/>
-      <c r="AD4" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AE4" s="13"/>
-      <c r="AF4" s="13"/>
-      <c r="AG4" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AH4" s="13"/>
-      <c r="AI4" s="17"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6">
+        <v>1</v>
+      </c>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6">
+        <v>0</v>
+      </c>
+      <c r="W4" s="6">
+        <v>1</v>
+      </c>
+      <c r="X4" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="Y4" s="6"/>
+      <c r="Z4" s="6"/>
+      <c r="AA4" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB4" s="6"/>
+      <c r="AC4" s="6"/>
+      <c r="AD4" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AE4" s="6"/>
+      <c r="AF4" s="6"/>
+      <c r="AG4" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AH4" s="6"/>
+      <c r="AI4" s="7"/>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="13">
-        <v>0</v>
-      </c>
-      <c r="I5" s="13" t="s">
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="6">
+        <v>0</v>
+      </c>
+      <c r="I5" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="J5" s="13">
+      <c r="J5" s="6">
         <v>0.1</v>
       </c>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="13"/>
-      <c r="R5" s="13"/>
-      <c r="S5" s="13">
-        <v>1</v>
-      </c>
-      <c r="T5" s="13"/>
-      <c r="U5" s="13"/>
-      <c r="V5" s="13">
-        <v>0</v>
-      </c>
-      <c r="W5" s="13">
-        <v>0</v>
-      </c>
-      <c r="X5" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="Y5" s="13"/>
-      <c r="Z5" s="13"/>
-      <c r="AA5" s="13">
-        <v>0</v>
-      </c>
-      <c r="AB5" s="13"/>
-      <c r="AC5" s="13"/>
-      <c r="AD5" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AE5" s="13"/>
-      <c r="AF5" s="13"/>
-      <c r="AG5" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AH5" s="13"/>
-      <c r="AI5" s="17"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6">
+        <v>1</v>
+      </c>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6">
+        <v>0</v>
+      </c>
+      <c r="W5" s="6">
+        <v>1</v>
+      </c>
+      <c r="X5" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="6"/>
+      <c r="AA5" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB5" s="6"/>
+      <c r="AC5" s="6"/>
+      <c r="AD5" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AE5" s="6"/>
+      <c r="AF5" s="6"/>
+      <c r="AG5" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AH5" s="6"/>
+      <c r="AI5" s="7"/>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="13">
-        <v>0</v>
-      </c>
-      <c r="I6" s="13" t="s">
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="6">
+        <v>0</v>
+      </c>
+      <c r="I6" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J6" s="13">
+      <c r="J6" s="6">
         <v>0.06</v>
       </c>
-      <c r="K6" s="13">
+      <c r="K6" s="6">
         <v>0.14000000000000001</v>
       </c>
-      <c r="L6" s="13"/>
-      <c r="M6" s="13"/>
-      <c r="N6" s="13"/>
-      <c r="O6" s="13"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="13"/>
-      <c r="R6" s="13"/>
-      <c r="S6" s="13">
-        <v>1</v>
-      </c>
-      <c r="T6" s="13"/>
-      <c r="U6" s="13"/>
-      <c r="V6" s="13">
-        <v>0</v>
-      </c>
-      <c r="W6" s="13">
-        <v>0</v>
-      </c>
-      <c r="X6" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="Y6" s="13"/>
-      <c r="Z6" s="13"/>
-      <c r="AA6" s="13">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="13"/>
-      <c r="AC6" s="13"/>
-      <c r="AD6" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AE6" s="13"/>
-      <c r="AF6" s="13"/>
-      <c r="AG6" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AH6" s="13"/>
-      <c r="AI6" s="17"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6">
+        <v>1</v>
+      </c>
+      <c r="T6" s="6"/>
+      <c r="U6" s="6"/>
+      <c r="V6" s="6">
+        <v>0</v>
+      </c>
+      <c r="W6" s="6">
+        <v>1</v>
+      </c>
+      <c r="X6" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="Y6" s="6"/>
+      <c r="Z6" s="6"/>
+      <c r="AA6" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB6" s="6"/>
+      <c r="AC6" s="6"/>
+      <c r="AD6" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AE6" s="6"/>
+      <c r="AF6" s="6"/>
+      <c r="AG6" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AH6" s="6"/>
+      <c r="AI6" s="7"/>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13" t="s">
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="H7" s="13">
-        <v>0</v>
-      </c>
-      <c r="I7" s="13" t="s">
+      <c r="H7" s="6">
+        <v>0</v>
+      </c>
+      <c r="I7" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J7" s="6">
         <v>0.08</v>
       </c>
-      <c r="K7" s="13">
+      <c r="K7" s="6">
         <v>0.15</v>
       </c>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13"/>
-      <c r="R7" s="13"/>
-      <c r="S7" s="13">
-        <v>1</v>
-      </c>
-      <c r="T7" s="13"/>
-      <c r="U7" s="13"/>
-      <c r="V7" s="13">
-        <v>0</v>
-      </c>
-      <c r="W7" s="13">
-        <v>0</v>
-      </c>
-      <c r="X7" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="Y7" s="13"/>
-      <c r="Z7" s="13"/>
-      <c r="AA7" s="13">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="13"/>
-      <c r="AC7" s="13"/>
-      <c r="AD7" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AE7" s="13"/>
-      <c r="AF7" s="13"/>
-      <c r="AG7" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AH7" s="13"/>
-      <c r="AI7" s="17"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6">
+        <v>1</v>
+      </c>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6">
+        <v>0</v>
+      </c>
+      <c r="W7" s="6">
+        <v>1</v>
+      </c>
+      <c r="X7" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="Y7" s="6"/>
+      <c r="Z7" s="6"/>
+      <c r="AA7" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB7" s="6"/>
+      <c r="AC7" s="6"/>
+      <c r="AD7" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AE7" s="6"/>
+      <c r="AF7" s="6"/>
+      <c r="AG7" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AH7" s="6"/>
+      <c r="AI7" s="7"/>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="13">
-        <v>0</v>
-      </c>
-      <c r="I8" s="13" t="s">
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="6">
+        <v>0</v>
+      </c>
+      <c r="I8" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J8" s="13">
+      <c r="J8" s="6">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="K8" s="13">
+      <c r="K8" s="6">
         <v>0.03</v>
       </c>
-      <c r="L8" s="13"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
-      <c r="P8" s="13"/>
-      <c r="Q8" s="13"/>
-      <c r="R8" s="13"/>
-      <c r="S8" s="13">
-        <v>1</v>
-      </c>
-      <c r="T8" s="13"/>
-      <c r="U8" s="13"/>
-      <c r="V8" s="13">
-        <v>0</v>
-      </c>
-      <c r="W8" s="13">
-        <v>0</v>
-      </c>
-      <c r="X8" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="Y8" s="13"/>
-      <c r="Z8" s="13"/>
-      <c r="AA8" s="13">
-        <v>0</v>
-      </c>
-      <c r="AB8" s="13"/>
-      <c r="AC8" s="13"/>
-      <c r="AD8" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AE8" s="13"/>
-      <c r="AF8" s="13"/>
-      <c r="AG8" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AH8" s="13"/>
-      <c r="AI8" s="17"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6">
+        <v>1</v>
+      </c>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6">
+        <v>0</v>
+      </c>
+      <c r="W8" s="6">
+        <v>1</v>
+      </c>
+      <c r="X8" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="Y8" s="6"/>
+      <c r="Z8" s="6"/>
+      <c r="AA8" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB8" s="6"/>
+      <c r="AC8" s="6"/>
+      <c r="AD8" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AE8" s="6"/>
+      <c r="AF8" s="6"/>
+      <c r="AG8" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AH8" s="6"/>
+      <c r="AI8" s="7"/>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13">
+      <c r="C9" s="6"/>
+      <c r="D9" s="6">
         <v>-0.05</v>
       </c>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13" t="s">
+      <c r="E9" s="6"/>
+      <c r="F9" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="G9" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="H9" s="13">
-        <v>0</v>
-      </c>
-      <c r="I9" s="13" t="s">
+      <c r="H9" s="6">
+        <v>0</v>
+      </c>
+      <c r="I9" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J9" s="13">
+      <c r="J9" s="6">
         <v>0.08</v>
       </c>
-      <c r="K9" s="13">
+      <c r="K9" s="6">
         <v>0.03</v>
       </c>
-      <c r="L9" s="13"/>
-      <c r="M9" s="13"/>
-      <c r="N9" s="13"/>
-      <c r="O9" s="13"/>
-      <c r="P9" s="13"/>
-      <c r="Q9" s="13"/>
-      <c r="R9" s="13"/>
-      <c r="S9" s="13">
-        <v>1</v>
-      </c>
-      <c r="T9" s="13"/>
-      <c r="U9" s="13"/>
-      <c r="V9" s="13">
-        <v>0</v>
-      </c>
-      <c r="W9" s="13">
-        <v>0</v>
-      </c>
-      <c r="X9" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="Y9" s="13"/>
-      <c r="Z9" s="13"/>
-      <c r="AA9" s="13">
-        <v>0</v>
-      </c>
-      <c r="AB9" s="13"/>
-      <c r="AC9" s="13"/>
-      <c r="AD9" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AE9" s="13"/>
-      <c r="AF9" s="13"/>
-      <c r="AG9" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AH9" s="13"/>
-      <c r="AI9" s="17"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6">
+        <v>1</v>
+      </c>
+      <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="6">
+        <v>0</v>
+      </c>
+      <c r="W9" s="6">
+        <v>1</v>
+      </c>
+      <c r="X9" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="Y9" s="6"/>
+      <c r="Z9" s="6"/>
+      <c r="AA9" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB9" s="6"/>
+      <c r="AC9" s="6"/>
+      <c r="AD9" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AE9" s="6"/>
+      <c r="AF9" s="6"/>
+      <c r="AG9" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AH9" s="6"/>
+      <c r="AI9" s="7"/>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="6">
         <v>0.01</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="6">
         <v>-0.05</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="6">
         <v>0.02</v>
       </c>
-      <c r="F10" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="13">
-        <v>1</v>
-      </c>
-      <c r="I10" s="13" t="s">
+      <c r="F10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="6">
+        <v>1</v>
+      </c>
+      <c r="I10" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="J10" s="13">
+      <c r="J10" s="6">
         <v>5.5E-2</v>
       </c>
-      <c r="K10" s="13"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="13"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="13"/>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="13"/>
-      <c r="R10" s="13"/>
-      <c r="S10" s="13">
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6">
         <v>0.1</v>
       </c>
-      <c r="T10" s="13"/>
-      <c r="U10" s="13"/>
-      <c r="V10" s="13">
-        <v>0</v>
-      </c>
-      <c r="W10" s="13">
-        <v>0</v>
-      </c>
-      <c r="X10" s="13">
-        <v>0</v>
-      </c>
-      <c r="Y10" s="13"/>
-      <c r="Z10" s="13"/>
-      <c r="AA10" s="13" t="s">
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="6">
+        <v>0</v>
+      </c>
+      <c r="W10" s="6">
+        <v>1</v>
+      </c>
+      <c r="X10" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="6"/>
+      <c r="Z10" s="6"/>
+      <c r="AA10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="AB10" s="13"/>
-      <c r="AC10" s="13"/>
-      <c r="AD10" s="13">
+      <c r="AB10" s="6"/>
+      <c r="AC10" s="6"/>
+      <c r="AD10" s="6">
         <v>0.9</v>
       </c>
-      <c r="AE10" s="13"/>
-      <c r="AF10" s="13"/>
-      <c r="AG10" s="13">
+      <c r="AE10" s="6"/>
+      <c r="AF10" s="6"/>
+      <c r="AG10" s="6">
         <v>0.95</v>
       </c>
-      <c r="AH10" s="13"/>
-      <c r="AI10" s="17"/>
+      <c r="AH10" s="6"/>
+      <c r="AI10" s="7"/>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C11" s="6">
         <v>-0.01</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="6">
         <v>-0.05</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="6">
         <v>0.02</v>
       </c>
-      <c r="F11" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G11" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" s="13">
-        <v>1</v>
-      </c>
-      <c r="I11" s="13" t="s">
+      <c r="F11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="6">
+        <v>1</v>
+      </c>
+      <c r="I11" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="J11" s="13">
+      <c r="J11" s="6">
         <v>5.5E-2</v>
       </c>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="13"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="13"/>
-      <c r="P11" s="13"/>
-      <c r="Q11" s="13"/>
-      <c r="R11" s="13"/>
-      <c r="S11" s="13">
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6">
         <v>0.1</v>
       </c>
-      <c r="T11" s="13"/>
-      <c r="U11" s="13"/>
-      <c r="V11" s="13">
-        <v>0</v>
-      </c>
-      <c r="W11" s="13">
-        <v>0</v>
-      </c>
-      <c r="X11" s="13">
-        <v>0</v>
-      </c>
-      <c r="Y11" s="13"/>
-      <c r="Z11" s="13"/>
-      <c r="AA11" s="13" t="s">
+      <c r="T11" s="6"/>
+      <c r="U11" s="6"/>
+      <c r="V11" s="6">
+        <v>0</v>
+      </c>
+      <c r="W11" s="6">
+        <v>1</v>
+      </c>
+      <c r="X11" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="6"/>
+      <c r="Z11" s="6"/>
+      <c r="AA11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="AB11" s="13"/>
-      <c r="AC11" s="13"/>
-      <c r="AD11" s="13">
+      <c r="AB11" s="6"/>
+      <c r="AC11" s="6"/>
+      <c r="AD11" s="6">
         <v>0.9</v>
       </c>
-      <c r="AE11" s="13"/>
-      <c r="AF11" s="13"/>
-      <c r="AG11" s="13">
+      <c r="AE11" s="6"/>
+      <c r="AF11" s="6"/>
+      <c r="AG11" s="6">
         <v>0.95</v>
       </c>
-      <c r="AH11" s="13"/>
-      <c r="AI11" s="17"/>
+      <c r="AH11" s="6"/>
+      <c r="AI11" s="7"/>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="13">
-        <v>0</v>
-      </c>
-      <c r="I12" s="13" t="s">
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="6">
+        <v>0</v>
+      </c>
+      <c r="I12" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J12" s="13">
+      <c r="J12" s="6">
         <v>0.1</v>
       </c>
-      <c r="K12" s="13">
+      <c r="K12" s="6">
         <v>0.08</v>
       </c>
-      <c r="L12" s="13"/>
-      <c r="M12" s="13"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="13"/>
-      <c r="P12" s="13"/>
-      <c r="Q12" s="13"/>
-      <c r="R12" s="13"/>
-      <c r="S12" s="13">
-        <v>1</v>
-      </c>
-      <c r="T12" s="13"/>
-      <c r="U12" s="13"/>
-      <c r="V12" s="13">
-        <v>0</v>
-      </c>
-      <c r="W12" s="13">
-        <v>0</v>
-      </c>
-      <c r="X12" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="Y12" s="13"/>
-      <c r="Z12" s="13"/>
-      <c r="AA12" s="13">
-        <v>0</v>
-      </c>
-      <c r="AB12" s="13"/>
-      <c r="AC12" s="13"/>
-      <c r="AD12" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AE12" s="13"/>
-      <c r="AF12" s="13"/>
-      <c r="AG12" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AH12" s="13"/>
-      <c r="AI12" s="17"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6">
+        <v>1</v>
+      </c>
+      <c r="T12" s="6"/>
+      <c r="U12" s="6"/>
+      <c r="V12" s="6">
+        <v>0</v>
+      </c>
+      <c r="W12" s="6">
+        <v>1</v>
+      </c>
+      <c r="X12" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="Y12" s="6"/>
+      <c r="Z12" s="6"/>
+      <c r="AA12" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB12" s="6"/>
+      <c r="AC12" s="6"/>
+      <c r="AD12" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AE12" s="6"/>
+      <c r="AF12" s="6"/>
+      <c r="AG12" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AH12" s="6"/>
+      <c r="AI12" s="7"/>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G13" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H13" s="13">
-        <v>0</v>
-      </c>
-      <c r="I13" s="13" t="s">
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" s="6">
+        <v>0</v>
+      </c>
+      <c r="I13" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J13" s="13">
+      <c r="J13" s="6">
         <v>0.09</v>
       </c>
-      <c r="K13" s="13">
+      <c r="K13" s="6">
         <v>0.28000000000000003</v>
       </c>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13"/>
-      <c r="O13" s="13"/>
-      <c r="P13" s="13"/>
-      <c r="Q13" s="13"/>
-      <c r="R13" s="13"/>
-      <c r="S13" s="13">
-        <v>1</v>
-      </c>
-      <c r="T13" s="13"/>
-      <c r="U13" s="13"/>
-      <c r="V13" s="13">
-        <v>0</v>
-      </c>
-      <c r="W13" s="13">
-        <v>0</v>
-      </c>
-      <c r="X13" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="Y13" s="13"/>
-      <c r="Z13" s="13"/>
-      <c r="AA13" s="13">
-        <v>0</v>
-      </c>
-      <c r="AB13" s="13"/>
-      <c r="AC13" s="13"/>
-      <c r="AD13" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AE13" s="13"/>
-      <c r="AF13" s="13"/>
-      <c r="AG13" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AH13" s="13"/>
-      <c r="AI13" s="17"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6">
+        <v>1</v>
+      </c>
+      <c r="T13" s="6"/>
+      <c r="U13" s="6"/>
+      <c r="V13" s="6">
+        <v>0</v>
+      </c>
+      <c r="W13" s="6">
+        <v>0</v>
+      </c>
+      <c r="X13" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="Y13" s="6"/>
+      <c r="Z13" s="6"/>
+      <c r="AA13" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB13" s="6"/>
+      <c r="AC13" s="6"/>
+      <c r="AD13" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AE13" s="6"/>
+      <c r="AF13" s="6"/>
+      <c r="AG13" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AH13" s="6"/>
+      <c r="AI13" s="7"/>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" s="13">
-        <v>0</v>
-      </c>
-      <c r="I14" s="13" t="s">
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="6">
+        <v>0</v>
+      </c>
+      <c r="I14" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J14" s="13">
+      <c r="J14" s="6">
         <v>0.09</v>
       </c>
-      <c r="K14" s="13">
+      <c r="K14" s="6">
         <v>0.28000000000000003</v>
       </c>
-      <c r="L14" s="13"/>
-      <c r="M14" s="13"/>
-      <c r="N14" s="13"/>
-      <c r="O14" s="13"/>
-      <c r="P14" s="13"/>
-      <c r="Q14" s="13"/>
-      <c r="R14" s="13"/>
-      <c r="S14" s="13">
-        <v>1</v>
-      </c>
-      <c r="T14" s="13"/>
-      <c r="U14" s="13"/>
-      <c r="V14" s="13">
-        <v>0</v>
-      </c>
-      <c r="W14" s="13">
-        <v>0</v>
-      </c>
-      <c r="X14" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="Y14" s="13"/>
-      <c r="Z14" s="13"/>
-      <c r="AA14" s="13">
-        <v>0</v>
-      </c>
-      <c r="AB14" s="13"/>
-      <c r="AC14" s="13"/>
-      <c r="AD14" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AE14" s="13"/>
-      <c r="AF14" s="13"/>
-      <c r="AG14" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AH14" s="13"/>
-      <c r="AI14" s="17"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
+      <c r="Q14" s="6"/>
+      <c r="R14" s="6"/>
+      <c r="S14" s="6">
+        <v>1</v>
+      </c>
+      <c r="T14" s="6"/>
+      <c r="U14" s="6"/>
+      <c r="V14" s="6">
+        <v>0</v>
+      </c>
+      <c r="W14" s="6">
+        <v>0</v>
+      </c>
+      <c r="X14" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="Y14" s="6"/>
+      <c r="Z14" s="6"/>
+      <c r="AA14" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB14" s="6"/>
+      <c r="AC14" s="6"/>
+      <c r="AD14" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AE14" s="6"/>
+      <c r="AF14" s="6"/>
+      <c r="AG14" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AH14" s="6"/>
+      <c r="AI14" s="7"/>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G15" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H15" s="13">
-        <v>0</v>
-      </c>
-      <c r="I15" s="13" t="s">
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" s="6">
+        <v>0</v>
+      </c>
+      <c r="I15" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J15" s="13">
+      <c r="J15" s="6">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="K15" s="13">
+      <c r="K15" s="6">
         <v>2.6499999999999999E-2</v>
       </c>
-      <c r="L15" s="13"/>
-      <c r="M15" s="13"/>
-      <c r="N15" s="13"/>
-      <c r="O15" s="13"/>
-      <c r="P15" s="13"/>
-      <c r="Q15" s="13"/>
-      <c r="R15" s="13"/>
-      <c r="S15" s="13">
-        <v>1</v>
-      </c>
-      <c r="T15" s="13"/>
-      <c r="U15" s="13"/>
-      <c r="V15" s="13">
-        <v>0</v>
-      </c>
-      <c r="W15" s="13">
-        <v>0</v>
-      </c>
-      <c r="X15" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="Y15" s="13"/>
-      <c r="Z15" s="13"/>
-      <c r="AA15" s="13">
-        <v>0</v>
-      </c>
-      <c r="AB15" s="13"/>
-      <c r="AC15" s="13"/>
-      <c r="AD15" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AE15" s="13"/>
-      <c r="AF15" s="13"/>
-      <c r="AG15" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AH15" s="13"/>
-      <c r="AI15" s="17"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
+      <c r="Q15" s="6"/>
+      <c r="R15" s="6"/>
+      <c r="S15" s="6">
+        <v>1</v>
+      </c>
+      <c r="T15" s="6"/>
+      <c r="U15" s="6"/>
+      <c r="V15" s="6">
+        <v>0</v>
+      </c>
+      <c r="W15" s="6">
+        <v>0</v>
+      </c>
+      <c r="X15" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="Y15" s="6"/>
+      <c r="Z15" s="6"/>
+      <c r="AA15" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB15" s="6"/>
+      <c r="AC15" s="6"/>
+      <c r="AD15" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AE15" s="6"/>
+      <c r="AF15" s="6"/>
+      <c r="AG15" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AH15" s="6"/>
+      <c r="AI15" s="7"/>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G16" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H16" s="13">
-        <v>0</v>
-      </c>
-      <c r="I16" s="13" t="s">
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" s="6">
+        <v>0</v>
+      </c>
+      <c r="I16" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J16" s="13">
+      <c r="J16" s="6">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="K16" s="13">
+      <c r="K16" s="6">
         <v>2.6499999999999999E-2</v>
       </c>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
-      <c r="N16" s="13"/>
-      <c r="O16" s="13"/>
-      <c r="P16" s="13"/>
-      <c r="Q16" s="13"/>
-      <c r="R16" s="13"/>
-      <c r="S16" s="13">
-        <v>1</v>
-      </c>
-      <c r="T16" s="13"/>
-      <c r="U16" s="13"/>
-      <c r="V16" s="13">
-        <v>0</v>
-      </c>
-      <c r="W16" s="13">
-        <v>0</v>
-      </c>
-      <c r="X16" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="Y16" s="13"/>
-      <c r="Z16" s="13"/>
-      <c r="AA16" s="13">
-        <v>0</v>
-      </c>
-      <c r="AB16" s="13"/>
-      <c r="AC16" s="13"/>
-      <c r="AD16" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AE16" s="13"/>
-      <c r="AF16" s="13"/>
-      <c r="AG16" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AH16" s="13"/>
-      <c r="AI16" s="17"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
+      <c r="Q16" s="6"/>
+      <c r="R16" s="6"/>
+      <c r="S16" s="6">
+        <v>1</v>
+      </c>
+      <c r="T16" s="6"/>
+      <c r="U16" s="6"/>
+      <c r="V16" s="6">
+        <v>0</v>
+      </c>
+      <c r="W16" s="6">
+        <v>0</v>
+      </c>
+      <c r="X16" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="Y16" s="6"/>
+      <c r="Z16" s="6"/>
+      <c r="AA16" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB16" s="6"/>
+      <c r="AC16" s="6"/>
+      <c r="AD16" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AE16" s="6"/>
+      <c r="AF16" s="6"/>
+      <c r="AG16" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AH16" s="6"/>
+      <c r="AI16" s="7"/>
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G17" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H17" s="13">
-        <v>0</v>
-      </c>
-      <c r="I17" s="13" t="s">
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" s="6">
+        <v>0</v>
+      </c>
+      <c r="I17" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J17" s="13">
+      <c r="J17" s="6">
         <v>0.06</v>
       </c>
-      <c r="K17" s="13">
+      <c r="K17" s="6">
         <v>0.4</v>
       </c>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-      <c r="N17" s="13"/>
-      <c r="O17" s="13"/>
-      <c r="P17" s="13"/>
-      <c r="Q17" s="13"/>
-      <c r="R17" s="13"/>
-      <c r="S17" s="13">
-        <v>1</v>
-      </c>
-      <c r="T17" s="13"/>
-      <c r="U17" s="13"/>
-      <c r="V17" s="13">
-        <v>0</v>
-      </c>
-      <c r="W17" s="13">
-        <v>0</v>
-      </c>
-      <c r="X17" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="Y17" s="13"/>
-      <c r="Z17" s="13"/>
-      <c r="AA17" s="13">
-        <v>0</v>
-      </c>
-      <c r="AB17" s="13"/>
-      <c r="AC17" s="13"/>
-      <c r="AD17" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AE17" s="13"/>
-      <c r="AF17" s="13"/>
-      <c r="AG17" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AH17" s="13"/>
-      <c r="AI17" s="17"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6">
+        <v>1</v>
+      </c>
+      <c r="T17" s="6"/>
+      <c r="U17" s="6"/>
+      <c r="V17" s="6">
+        <v>0</v>
+      </c>
+      <c r="W17" s="6">
+        <v>0</v>
+      </c>
+      <c r="X17" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="Y17" s="6"/>
+      <c r="Z17" s="6"/>
+      <c r="AA17" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB17" s="6"/>
+      <c r="AC17" s="6"/>
+      <c r="AD17" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AE17" s="6"/>
+      <c r="AF17" s="6"/>
+      <c r="AG17" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AH17" s="6"/>
+      <c r="AI17" s="7"/>
     </row>
     <row r="18" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G18" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H18" s="13">
-        <v>0</v>
-      </c>
-      <c r="I18" s="13" t="s">
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" s="6">
+        <v>0</v>
+      </c>
+      <c r="I18" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J18" s="13">
+      <c r="J18" s="6">
         <v>0.06</v>
       </c>
-      <c r="K18" s="13">
+      <c r="K18" s="6">
         <v>0.4</v>
       </c>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="13"/>
-      <c r="O18" s="13"/>
-      <c r="P18" s="13"/>
-      <c r="Q18" s="13"/>
-      <c r="R18" s="13"/>
-      <c r="S18" s="13">
-        <v>1</v>
-      </c>
-      <c r="T18" s="13"/>
-      <c r="U18" s="13"/>
-      <c r="V18" s="13">
-        <v>0</v>
-      </c>
-      <c r="W18" s="13">
-        <v>0</v>
-      </c>
-      <c r="X18" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="Y18" s="13"/>
-      <c r="Z18" s="13"/>
-      <c r="AA18" s="13">
-        <v>0</v>
-      </c>
-      <c r="AB18" s="13"/>
-      <c r="AC18" s="13"/>
-      <c r="AD18" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AE18" s="13"/>
-      <c r="AF18" s="13"/>
-      <c r="AG18" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AH18" s="13"/>
-      <c r="AI18" s="17"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
+      <c r="Q18" s="6"/>
+      <c r="R18" s="6"/>
+      <c r="S18" s="6">
+        <v>1</v>
+      </c>
+      <c r="T18" s="6"/>
+      <c r="U18" s="6"/>
+      <c r="V18" s="6">
+        <v>0</v>
+      </c>
+      <c r="W18" s="6">
+        <v>0</v>
+      </c>
+      <c r="X18" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="Y18" s="6"/>
+      <c r="Z18" s="6"/>
+      <c r="AA18" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB18" s="6"/>
+      <c r="AC18" s="6"/>
+      <c r="AD18" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AE18" s="6"/>
+      <c r="AF18" s="6"/>
+      <c r="AG18" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AH18" s="6"/>
+      <c r="AI18" s="7"/>
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G19" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H19" s="13">
-        <v>0</v>
-      </c>
-      <c r="I19" s="13" t="s">
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19" s="6">
+        <v>0</v>
+      </c>
+      <c r="I19" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J19" s="13">
+      <c r="J19" s="6">
         <v>0.04</v>
       </c>
-      <c r="K19" s="13">
+      <c r="K19" s="6">
         <v>0.13</v>
       </c>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
-      <c r="O19" s="13"/>
-      <c r="P19" s="13"/>
-      <c r="Q19" s="13"/>
-      <c r="R19" s="13"/>
-      <c r="S19" s="13">
-        <v>1</v>
-      </c>
-      <c r="T19" s="13"/>
-      <c r="U19" s="13"/>
-      <c r="V19" s="13">
-        <v>0</v>
-      </c>
-      <c r="W19" s="13">
-        <v>0</v>
-      </c>
-      <c r="X19" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="Y19" s="13"/>
-      <c r="Z19" s="13"/>
-      <c r="AA19" s="13">
-        <v>0</v>
-      </c>
-      <c r="AB19" s="13"/>
-      <c r="AC19" s="13"/>
-      <c r="AD19" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AE19" s="13"/>
-      <c r="AF19" s="13"/>
-      <c r="AG19" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AH19" s="13"/>
-      <c r="AI19" s="17"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
+      <c r="Q19" s="6"/>
+      <c r="R19" s="6"/>
+      <c r="S19" s="6">
+        <v>1</v>
+      </c>
+      <c r="T19" s="6"/>
+      <c r="U19" s="6"/>
+      <c r="V19" s="6">
+        <v>0</v>
+      </c>
+      <c r="W19" s="6">
+        <v>0</v>
+      </c>
+      <c r="X19" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="Y19" s="6"/>
+      <c r="Z19" s="6"/>
+      <c r="AA19" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB19" s="6"/>
+      <c r="AC19" s="6"/>
+      <c r="AD19" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AE19" s="6"/>
+      <c r="AF19" s="6"/>
+      <c r="AG19" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AH19" s="6"/>
+      <c r="AI19" s="7"/>
     </row>
     <row r="20" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G20" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H20" s="13">
-        <v>0</v>
-      </c>
-      <c r="I20" s="13" t="s">
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" s="6">
+        <v>0</v>
+      </c>
+      <c r="I20" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J20" s="13">
+      <c r="J20" s="6">
         <v>0.04</v>
       </c>
-      <c r="K20" s="13">
+      <c r="K20" s="6">
         <v>0.13</v>
       </c>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
-      <c r="P20" s="13"/>
-      <c r="Q20" s="13"/>
-      <c r="R20" s="13"/>
-      <c r="S20" s="13">
-        <v>1</v>
-      </c>
-      <c r="T20" s="13"/>
-      <c r="U20" s="13"/>
-      <c r="V20" s="13">
-        <v>0</v>
-      </c>
-      <c r="W20" s="13">
-        <v>0</v>
-      </c>
-      <c r="X20" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="Y20" s="13"/>
-      <c r="Z20" s="13"/>
-      <c r="AA20" s="13">
-        <v>0</v>
-      </c>
-      <c r="AB20" s="13"/>
-      <c r="AC20" s="13"/>
-      <c r="AD20" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AE20" s="13"/>
-      <c r="AF20" s="13"/>
-      <c r="AG20" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AH20" s="13"/>
-      <c r="AI20" s="17"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="6"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="6">
+        <v>1</v>
+      </c>
+      <c r="T20" s="6"/>
+      <c r="U20" s="6"/>
+      <c r="V20" s="6">
+        <v>0</v>
+      </c>
+      <c r="W20" s="6">
+        <v>0</v>
+      </c>
+      <c r="X20" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="Y20" s="6"/>
+      <c r="Z20" s="6"/>
+      <c r="AA20" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB20" s="6"/>
+      <c r="AC20" s="6"/>
+      <c r="AD20" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AE20" s="6"/>
+      <c r="AF20" s="6"/>
+      <c r="AG20" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AH20" s="6"/>
+      <c r="AI20" s="7"/>
     </row>
     <row r="21" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G21" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H21" s="13">
-        <v>0</v>
-      </c>
-      <c r="I21" s="13" t="s">
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" s="6">
+        <v>0</v>
+      </c>
+      <c r="I21" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J21" s="13">
+      <c r="J21" s="6">
         <v>0.08</v>
       </c>
-      <c r="K21" s="13">
+      <c r="K21" s="6">
         <v>0.08</v>
       </c>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13"/>
-      <c r="P21" s="13"/>
-      <c r="Q21" s="13"/>
-      <c r="R21" s="13"/>
-      <c r="S21" s="13">
-        <v>1</v>
-      </c>
-      <c r="T21" s="13"/>
-      <c r="U21" s="13"/>
-      <c r="V21" s="13">
-        <v>0</v>
-      </c>
-      <c r="W21" s="13">
-        <v>0</v>
-      </c>
-      <c r="X21" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="Y21" s="13"/>
-      <c r="Z21" s="13"/>
-      <c r="AA21" s="13">
-        <v>0</v>
-      </c>
-      <c r="AB21" s="13"/>
-      <c r="AC21" s="13"/>
-      <c r="AD21" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AE21" s="13"/>
-      <c r="AF21" s="13"/>
-      <c r="AG21" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AH21" s="13"/>
-      <c r="AI21" s="17"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="6"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="6"/>
+      <c r="S21" s="6">
+        <v>1</v>
+      </c>
+      <c r="T21" s="6"/>
+      <c r="U21" s="6"/>
+      <c r="V21" s="6">
+        <v>0</v>
+      </c>
+      <c r="W21" s="6">
+        <v>0</v>
+      </c>
+      <c r="X21" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="Y21" s="6"/>
+      <c r="Z21" s="6"/>
+      <c r="AA21" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB21" s="6"/>
+      <c r="AC21" s="6"/>
+      <c r="AD21" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AE21" s="6"/>
+      <c r="AF21" s="6"/>
+      <c r="AG21" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AH21" s="6"/>
+      <c r="AI21" s="7"/>
     </row>
     <row r="22" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G22" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H22" s="13">
-        <v>0</v>
-      </c>
-      <c r="I22" s="13" t="s">
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22" s="6">
+        <v>0</v>
+      </c>
+      <c r="I22" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J22" s="13">
+      <c r="J22" s="6">
         <v>0.08</v>
       </c>
-      <c r="K22" s="13">
+      <c r="K22" s="6">
         <v>0.08</v>
       </c>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
-      <c r="P22" s="13"/>
-      <c r="Q22" s="13"/>
-      <c r="R22" s="13"/>
-      <c r="S22" s="13">
-        <v>1</v>
-      </c>
-      <c r="T22" s="13"/>
-      <c r="U22" s="13"/>
-      <c r="V22" s="13">
-        <v>0</v>
-      </c>
-      <c r="W22" s="13">
-        <v>0</v>
-      </c>
-      <c r="X22" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="Y22" s="13"/>
-      <c r="Z22" s="13"/>
-      <c r="AA22" s="13">
-        <v>0</v>
-      </c>
-      <c r="AB22" s="13"/>
-      <c r="AC22" s="13"/>
-      <c r="AD22" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AE22" s="13"/>
-      <c r="AF22" s="13"/>
-      <c r="AG22" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AH22" s="13"/>
-      <c r="AI22" s="17"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="6"/>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
+      <c r="P22" s="6"/>
+      <c r="Q22" s="6"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="6">
+        <v>1</v>
+      </c>
+      <c r="T22" s="6"/>
+      <c r="U22" s="6"/>
+      <c r="V22" s="6">
+        <v>0</v>
+      </c>
+      <c r="W22" s="6">
+        <v>0</v>
+      </c>
+      <c r="X22" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="Y22" s="6"/>
+      <c r="Z22" s="6"/>
+      <c r="AA22" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB22" s="6"/>
+      <c r="AC22" s="6"/>
+      <c r="AD22" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AE22" s="6"/>
+      <c r="AF22" s="6"/>
+      <c r="AG22" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AH22" s="6"/>
+      <c r="AI22" s="7"/>
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G23" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H23" s="13">
-        <v>0</v>
-      </c>
-      <c r="I23" s="13" t="s">
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H23" s="6">
+        <v>0</v>
+      </c>
+      <c r="I23" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J23" s="13">
+      <c r="J23" s="6">
         <v>0.06</v>
       </c>
-      <c r="K23" s="13">
+      <c r="K23" s="6">
         <v>0.28000000000000003</v>
       </c>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="13"/>
-      <c r="P23" s="13"/>
-      <c r="Q23" s="13"/>
-      <c r="R23" s="13"/>
-      <c r="S23" s="13">
-        <v>1</v>
-      </c>
-      <c r="T23" s="13"/>
-      <c r="U23" s="13"/>
-      <c r="V23" s="13">
-        <v>0</v>
-      </c>
-      <c r="W23" s="13">
-        <v>14</v>
-      </c>
-      <c r="X23" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="Y23" s="13"/>
-      <c r="Z23" s="13"/>
-      <c r="AA23" s="13">
-        <v>0</v>
-      </c>
-      <c r="AB23" s="13"/>
-      <c r="AC23" s="13"/>
-      <c r="AD23" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AE23" s="13"/>
-      <c r="AF23" s="13"/>
-      <c r="AG23" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AH23" s="13"/>
-      <c r="AI23" s="17"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="6"/>
+      <c r="Q23" s="6"/>
+      <c r="R23" s="6"/>
+      <c r="S23" s="6">
+        <v>1</v>
+      </c>
+      <c r="T23" s="6"/>
+      <c r="U23" s="6"/>
+      <c r="V23" s="6">
+        <v>0</v>
+      </c>
+      <c r="W23" s="6">
+        <v>0</v>
+      </c>
+      <c r="X23" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="Y23" s="6"/>
+      <c r="Z23" s="6"/>
+      <c r="AA23" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB23" s="6"/>
+      <c r="AC23" s="6"/>
+      <c r="AD23" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AE23" s="6"/>
+      <c r="AF23" s="6"/>
+      <c r="AG23" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AH23" s="6"/>
+      <c r="AI23" s="7"/>
     </row>
     <row r="24" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A24" s="14" t="s">
+      <c r="A24" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G24" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H24" s="13">
-        <v>0</v>
-      </c>
-      <c r="I24" s="13" t="s">
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H24" s="6">
+        <v>0</v>
+      </c>
+      <c r="I24" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J24" s="13">
+      <c r="J24" s="6">
         <v>0.06</v>
       </c>
-      <c r="K24" s="13">
+      <c r="K24" s="6">
         <v>0.28000000000000003</v>
       </c>
-      <c r="L24" s="13"/>
-      <c r="M24" s="13"/>
-      <c r="N24" s="13"/>
-      <c r="O24" s="13"/>
-      <c r="P24" s="13"/>
-      <c r="Q24" s="13"/>
-      <c r="R24" s="13"/>
-      <c r="S24" s="13">
-        <v>1</v>
-      </c>
-      <c r="T24" s="13"/>
-      <c r="U24" s="13"/>
-      <c r="V24" s="13">
-        <v>0</v>
-      </c>
-      <c r="W24" s="13">
-        <v>14</v>
-      </c>
-      <c r="X24" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="Y24" s="13"/>
-      <c r="Z24" s="13"/>
-      <c r="AA24" s="13">
-        <v>0</v>
-      </c>
-      <c r="AB24" s="13"/>
-      <c r="AC24" s="13"/>
-      <c r="AD24" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AE24" s="13"/>
-      <c r="AF24" s="13"/>
-      <c r="AG24" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AH24" s="13"/>
-      <c r="AI24" s="17"/>
+      <c r="L24" s="6"/>
+      <c r="M24" s="6"/>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
+      <c r="Q24" s="6"/>
+      <c r="R24" s="6"/>
+      <c r="S24" s="6">
+        <v>1</v>
+      </c>
+      <c r="T24" s="6"/>
+      <c r="U24" s="6"/>
+      <c r="V24" s="6">
+        <v>0</v>
+      </c>
+      <c r="W24" s="6">
+        <v>0</v>
+      </c>
+      <c r="X24" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="Y24" s="6"/>
+      <c r="Z24" s="6"/>
+      <c r="AA24" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB24" s="6"/>
+      <c r="AC24" s="6"/>
+      <c r="AD24" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AE24" s="6"/>
+      <c r="AF24" s="6"/>
+      <c r="AG24" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AH24" s="6"/>
+      <c r="AI24" s="7"/>
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
+      <c r="A25" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G25" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H25" s="13">
-        <v>0</v>
-      </c>
-      <c r="I25" s="13" t="s">
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25" s="6">
+        <v>0</v>
+      </c>
+      <c r="I25" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J25" s="13">
+      <c r="J25" s="6">
         <v>0.05</v>
       </c>
-      <c r="K25" s="13">
+      <c r="K25" s="6">
         <v>0.25</v>
       </c>
-      <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
-      <c r="N25" s="13"/>
-      <c r="O25" s="13"/>
-      <c r="P25" s="13"/>
-      <c r="Q25" s="13"/>
-      <c r="R25" s="13"/>
-      <c r="S25" s="13">
-        <v>1</v>
-      </c>
-      <c r="T25" s="13"/>
-      <c r="U25" s="13"/>
-      <c r="V25" s="13">
-        <v>0</v>
-      </c>
-      <c r="W25" s="13">
-        <v>0</v>
-      </c>
-      <c r="X25" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="Y25" s="13"/>
-      <c r="Z25" s="13"/>
-      <c r="AA25" s="13">
-        <v>0</v>
-      </c>
-      <c r="AB25" s="13"/>
-      <c r="AC25" s="13"/>
-      <c r="AD25" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AE25" s="13"/>
-      <c r="AF25" s="13"/>
-      <c r="AG25" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AH25" s="13"/>
-      <c r="AI25" s="17"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="6"/>
+      <c r="P25" s="6"/>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="6"/>
+      <c r="S25" s="6">
+        <v>1</v>
+      </c>
+      <c r="T25" s="6"/>
+      <c r="U25" s="6"/>
+      <c r="V25" s="6">
+        <v>0</v>
+      </c>
+      <c r="W25" s="6">
+        <v>0</v>
+      </c>
+      <c r="X25" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="Y25" s="6"/>
+      <c r="Z25" s="6"/>
+      <c r="AA25" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB25" s="6"/>
+      <c r="AC25" s="6"/>
+      <c r="AD25" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AE25" s="6"/>
+      <c r="AF25" s="6"/>
+      <c r="AG25" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AH25" s="6"/>
+      <c r="AI25" s="7"/>
     </row>
     <row r="26" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G26" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H26" s="13">
-        <v>0</v>
-      </c>
-      <c r="I26" s="13" t="s">
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H26" s="6">
+        <v>0</v>
+      </c>
+      <c r="I26" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J26" s="13">
+      <c r="J26" s="6">
         <v>0.05</v>
       </c>
-      <c r="K26" s="13">
+      <c r="K26" s="6">
         <v>0.25</v>
       </c>
-      <c r="L26" s="13"/>
-      <c r="M26" s="13"/>
-      <c r="N26" s="13"/>
-      <c r="O26" s="13"/>
-      <c r="P26" s="13"/>
-      <c r="Q26" s="13"/>
-      <c r="R26" s="13"/>
-      <c r="S26" s="13">
-        <v>1</v>
-      </c>
-      <c r="T26" s="13"/>
-      <c r="U26" s="13"/>
-      <c r="V26" s="13">
-        <v>0</v>
-      </c>
-      <c r="W26" s="13">
-        <v>0</v>
-      </c>
-      <c r="X26" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="Y26" s="13"/>
-      <c r="Z26" s="13"/>
-      <c r="AA26" s="13">
-        <v>0</v>
-      </c>
-      <c r="AB26" s="13"/>
-      <c r="AC26" s="13"/>
-      <c r="AD26" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AE26" s="13"/>
-      <c r="AF26" s="13"/>
-      <c r="AG26" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AH26" s="13"/>
-      <c r="AI26" s="17"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="6"/>
+      <c r="P26" s="6"/>
+      <c r="Q26" s="6"/>
+      <c r="R26" s="6"/>
+      <c r="S26" s="6">
+        <v>1</v>
+      </c>
+      <c r="T26" s="6"/>
+      <c r="U26" s="6"/>
+      <c r="V26" s="6">
+        <v>0</v>
+      </c>
+      <c r="W26" s="6">
+        <v>0</v>
+      </c>
+      <c r="X26" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="Y26" s="6"/>
+      <c r="Z26" s="6"/>
+      <c r="AA26" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB26" s="6"/>
+      <c r="AC26" s="6"/>
+      <c r="AD26" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AE26" s="6"/>
+      <c r="AF26" s="6"/>
+      <c r="AG26" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AH26" s="6"/>
+      <c r="AI26" s="7"/>
     </row>
     <row r="27" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G27" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H27" s="13">
-        <v>0</v>
-      </c>
-      <c r="I27" s="13" t="s">
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" s="6">
+        <v>0</v>
+      </c>
+      <c r="I27" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="J27" s="13">
+      <c r="J27" s="6">
         <v>0.04</v>
       </c>
-      <c r="K27" s="13">
+      <c r="K27" s="6">
         <v>0.01</v>
       </c>
-      <c r="L27" s="13">
+      <c r="L27" s="6">
         <v>0.04</v>
       </c>
-      <c r="M27" s="13"/>
-      <c r="N27" s="13"/>
-      <c r="O27" s="13"/>
-      <c r="P27" s="13"/>
-      <c r="Q27" s="13"/>
-      <c r="R27" s="13"/>
-      <c r="S27" s="13">
-        <v>1</v>
-      </c>
-      <c r="T27" s="13"/>
-      <c r="U27" s="13"/>
-      <c r="V27" s="13">
-        <v>0</v>
-      </c>
-      <c r="W27" s="13">
-        <v>0</v>
-      </c>
-      <c r="X27" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="Y27" s="13"/>
-      <c r="Z27" s="13"/>
-      <c r="AA27" s="13">
-        <v>0</v>
-      </c>
-      <c r="AB27" s="13"/>
-      <c r="AC27" s="13"/>
-      <c r="AD27" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AE27" s="13"/>
-      <c r="AF27" s="13"/>
-      <c r="AG27" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AH27" s="13"/>
-      <c r="AI27" s="17"/>
+      <c r="M27" s="6"/>
+      <c r="N27" s="6"/>
+      <c r="O27" s="6"/>
+      <c r="P27" s="6"/>
+      <c r="Q27" s="6"/>
+      <c r="R27" s="6"/>
+      <c r="S27" s="6">
+        <v>1</v>
+      </c>
+      <c r="T27" s="6"/>
+      <c r="U27" s="6"/>
+      <c r="V27" s="6">
+        <v>0</v>
+      </c>
+      <c r="W27" s="6">
+        <v>0</v>
+      </c>
+      <c r="X27" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="Y27" s="6"/>
+      <c r="Z27" s="6"/>
+      <c r="AA27" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB27" s="6"/>
+      <c r="AC27" s="6"/>
+      <c r="AD27" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AE27" s="6"/>
+      <c r="AF27" s="6"/>
+      <c r="AG27" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AH27" s="6"/>
+      <c r="AI27" s="7"/>
     </row>
     <row r="28" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G28" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H28" s="13">
-        <v>0</v>
-      </c>
-      <c r="I28" s="13" t="s">
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H28" s="6">
+        <v>0</v>
+      </c>
+      <c r="I28" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="J28" s="13">
+      <c r="J28" s="6">
         <v>0.04</v>
       </c>
-      <c r="K28" s="13">
+      <c r="K28" s="6">
         <v>0.01</v>
       </c>
-      <c r="L28" s="13">
+      <c r="L28" s="6">
         <v>0.04</v>
       </c>
-      <c r="M28" s="13"/>
-      <c r="N28" s="13"/>
-      <c r="O28" s="13"/>
-      <c r="P28" s="13"/>
-      <c r="Q28" s="13"/>
-      <c r="R28" s="13"/>
-      <c r="S28" s="13">
-        <v>1</v>
-      </c>
-      <c r="T28" s="13"/>
-      <c r="U28" s="13"/>
-      <c r="V28" s="13">
-        <v>0</v>
-      </c>
-      <c r="W28" s="13">
-        <v>0</v>
-      </c>
-      <c r="X28" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="Y28" s="13"/>
-      <c r="Z28" s="13"/>
-      <c r="AA28" s="13">
-        <v>0</v>
-      </c>
-      <c r="AB28" s="13"/>
-      <c r="AC28" s="13"/>
-      <c r="AD28" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AE28" s="13"/>
-      <c r="AF28" s="13"/>
-      <c r="AG28" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="AH28" s="13"/>
-      <c r="AI28" s="17"/>
+      <c r="M28" s="6"/>
+      <c r="N28" s="6"/>
+      <c r="O28" s="6"/>
+      <c r="P28" s="6"/>
+      <c r="Q28" s="6"/>
+      <c r="R28" s="6"/>
+      <c r="S28" s="6">
+        <v>1</v>
+      </c>
+      <c r="T28" s="6"/>
+      <c r="U28" s="6"/>
+      <c r="V28" s="6">
+        <v>0</v>
+      </c>
+      <c r="W28" s="6">
+        <v>0</v>
+      </c>
+      <c r="X28" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="Y28" s="6"/>
+      <c r="Z28" s="6"/>
+      <c r="AA28" t="s">
+        <v>114</v>
+      </c>
+      <c r="AB28" s="6"/>
+      <c r="AC28" s="6"/>
+      <c r="AD28" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AE28" s="6"/>
+      <c r="AF28" s="6"/>
+      <c r="AG28" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AH28" s="6"/>
+      <c r="AI28" s="7"/>
     </row>
     <row r="29" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G29" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H29" s="13">
-        <v>1</v>
-      </c>
-      <c r="I29" s="13" t="s">
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H29" s="6">
+        <v>1</v>
+      </c>
+      <c r="I29" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="J29" s="13">
+      <c r="J29" s="6">
         <v>0.03</v>
       </c>
-      <c r="K29" s="13">
+      <c r="K29" s="6">
         <v>0.01</v>
       </c>
-      <c r="L29" s="13">
+      <c r="L29" s="6">
         <v>0.05</v>
       </c>
-      <c r="M29" s="13"/>
-      <c r="N29" s="13"/>
-      <c r="O29" s="13"/>
-      <c r="P29" s="13"/>
-      <c r="Q29" s="13"/>
-      <c r="R29" s="13"/>
-      <c r="S29" s="13"/>
-      <c r="T29" s="13">
+      <c r="M29" s="6"/>
+      <c r="N29" s="6"/>
+      <c r="O29" s="6"/>
+      <c r="P29" s="6"/>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="6"/>
+      <c r="S29" s="6"/>
+      <c r="T29" s="6">
         <v>5</v>
       </c>
-      <c r="U29" s="13">
+      <c r="U29" s="6">
         <v>10</v>
       </c>
-      <c r="V29" s="13">
-        <v>0</v>
-      </c>
-      <c r="W29" s="13">
+      <c r="V29" s="6">
+        <v>0</v>
+      </c>
+      <c r="W29" s="6">
         <v>10</v>
       </c>
-      <c r="X29" s="13"/>
-      <c r="Y29" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="Z29" s="13">
-        <v>1</v>
-      </c>
-      <c r="AA29" s="19" t="s">
+      <c r="X29" s="6"/>
+      <c r="Y29" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="Z29" s="6">
+        <v>1</v>
+      </c>
+      <c r="AA29" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="AB29" s="19"/>
-      <c r="AC29" s="19"/>
-      <c r="AD29" s="13"/>
-      <c r="AE29" s="13">
+      <c r="AB29" s="13"/>
+      <c r="AC29" s="13"/>
+      <c r="AD29" s="6"/>
+      <c r="AE29" s="6">
         <v>0.995</v>
       </c>
-      <c r="AF29" s="13">
-        <v>1</v>
-      </c>
-      <c r="AG29" s="13"/>
-      <c r="AH29" s="13">
+      <c r="AF29" s="6">
+        <v>1</v>
+      </c>
+      <c r="AG29" s="6"/>
+      <c r="AH29" s="6">
         <v>0.89</v>
       </c>
-      <c r="AI29" s="17">
+      <c r="AI29" s="7">
         <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A30" s="14" t="s">
+      <c r="A30" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G30" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H30" s="13">
-        <v>1</v>
-      </c>
-      <c r="I30" s="13" t="s">
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H30" s="6">
+        <v>1</v>
+      </c>
+      <c r="I30" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="J30" s="13">
+      <c r="J30" s="6">
         <v>0.03</v>
       </c>
-      <c r="K30" s="13">
+      <c r="K30" s="6">
         <v>0.04</v>
       </c>
-      <c r="L30" s="13"/>
-      <c r="M30" s="13"/>
-      <c r="N30" s="13"/>
-      <c r="O30" s="13"/>
-      <c r="P30" s="13"/>
-      <c r="Q30" s="13"/>
-      <c r="R30" s="13"/>
-      <c r="S30" s="13"/>
-      <c r="T30" s="13">
+      <c r="L30" s="6"/>
+      <c r="M30" s="6"/>
+      <c r="N30" s="6"/>
+      <c r="O30" s="6"/>
+      <c r="P30" s="6"/>
+      <c r="Q30" s="6"/>
+      <c r="R30" s="6"/>
+      <c r="S30" s="6"/>
+      <c r="T30" s="6">
         <v>10</v>
       </c>
-      <c r="U30" s="13">
+      <c r="U30" s="6">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="V30" s="13">
-        <v>0</v>
-      </c>
-      <c r="W30" s="13">
+      <c r="V30" s="6">
+        <v>0</v>
+      </c>
+      <c r="W30" s="6">
         <v>8</v>
       </c>
-      <c r="X30" s="13"/>
-      <c r="Y30" s="13">
+      <c r="X30" s="6"/>
+      <c r="Y30" s="6">
         <v>0.6</v>
       </c>
-      <c r="Z30" s="13">
+      <c r="Z30" s="6">
         <v>0.45</v>
       </c>
-      <c r="AA30" s="13"/>
-      <c r="AB30" s="13"/>
-      <c r="AC30" s="13"/>
-      <c r="AD30" s="13"/>
-      <c r="AE30" s="13"/>
-      <c r="AF30" s="13"/>
-      <c r="AG30" s="13"/>
-      <c r="AH30" s="13"/>
-      <c r="AI30" s="17"/>
+      <c r="AA30" s="6"/>
+      <c r="AB30" s="6"/>
+      <c r="AC30" s="6"/>
+      <c r="AD30" s="6"/>
+      <c r="AE30" s="6"/>
+      <c r="AF30" s="6"/>
+      <c r="AG30" s="6"/>
+      <c r="AH30" s="6"/>
+      <c r="AI30" s="7"/>
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A31" s="14" t="s">
+      <c r="A31" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G31" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H31" s="13">
-        <v>1</v>
-      </c>
-      <c r="I31" s="13" t="s">
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H31" s="6">
+        <v>1</v>
+      </c>
+      <c r="I31" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="J31" s="13">
+      <c r="J31" s="6">
         <v>0.02</v>
       </c>
-      <c r="K31" s="13">
+      <c r="K31" s="6">
         <v>0.09</v>
       </c>
-      <c r="L31" s="13">
+      <c r="L31" s="6">
         <v>0.04</v>
       </c>
-      <c r="M31" s="13"/>
-      <c r="N31" s="13"/>
-      <c r="O31" s="13"/>
-      <c r="P31" s="13"/>
-      <c r="Q31" s="13"/>
-      <c r="R31" s="13"/>
-      <c r="S31" s="13">
+      <c r="M31" s="6"/>
+      <c r="N31" s="6"/>
+      <c r="O31" s="6"/>
+      <c r="P31" s="6"/>
+      <c r="Q31" s="6"/>
+      <c r="R31" s="6"/>
+      <c r="S31" s="6">
         <v>10</v>
       </c>
-      <c r="T31" s="13"/>
-      <c r="U31" s="13"/>
-      <c r="V31" s="13">
-        <v>0</v>
-      </c>
-      <c r="W31" s="13">
+      <c r="T31" s="6"/>
+      <c r="U31" s="6"/>
+      <c r="V31" s="6">
+        <v>0</v>
+      </c>
+      <c r="W31" s="6">
         <v>4</v>
       </c>
-      <c r="X31" s="13">
+      <c r="X31" s="6">
         <v>0.6</v>
       </c>
-      <c r="Y31" s="13"/>
-      <c r="Z31" s="13"/>
-      <c r="AA31" s="13" t="s">
+      <c r="Y31" s="6"/>
+      <c r="Z31" s="6"/>
+      <c r="AA31" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="AB31" s="13"/>
-      <c r="AC31" s="13"/>
-      <c r="AD31" s="13">
-        <v>1</v>
-      </c>
-      <c r="AE31" s="13"/>
-      <c r="AF31" s="13"/>
-      <c r="AG31" s="13">
-        <v>1</v>
-      </c>
-      <c r="AH31" s="13"/>
-      <c r="AI31" s="17"/>
+      <c r="AB31" s="6"/>
+      <c r="AC31" s="6"/>
+      <c r="AD31" s="6">
+        <v>1</v>
+      </c>
+      <c r="AE31" s="6"/>
+      <c r="AF31" s="6"/>
+      <c r="AG31" s="6">
+        <v>1</v>
+      </c>
+      <c r="AH31" s="6"/>
+      <c r="AI31" s="7"/>
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="B32" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G32" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H32" s="13">
-        <v>1</v>
-      </c>
-      <c r="I32" s="13" t="s">
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H32" s="6">
+        <v>1</v>
+      </c>
+      <c r="I32" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="J32" s="13">
+      <c r="J32" s="6">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="K32" s="13">
+      <c r="K32" s="6">
         <v>0.05</v>
       </c>
-      <c r="L32" s="13">
+      <c r="L32" s="6">
         <v>0.05</v>
       </c>
-      <c r="M32" s="13"/>
-      <c r="N32" s="13"/>
-      <c r="O32" s="13"/>
-      <c r="P32" s="13"/>
-      <c r="Q32" s="13"/>
-      <c r="R32" s="13"/>
-      <c r="S32" s="13">
+      <c r="M32" s="6"/>
+      <c r="N32" s="6"/>
+      <c r="O32" s="6"/>
+      <c r="P32" s="6"/>
+      <c r="Q32" s="6"/>
+      <c r="R32" s="6"/>
+      <c r="S32" s="6">
         <v>5</v>
       </c>
-      <c r="T32" s="13"/>
-      <c r="U32" s="13"/>
-      <c r="V32" s="13">
-        <v>0</v>
-      </c>
-      <c r="W32" s="13">
+      <c r="T32" s="6"/>
+      <c r="U32" s="6"/>
+      <c r="V32" s="6">
+        <v>0</v>
+      </c>
+      <c r="W32" s="6">
         <v>4</v>
       </c>
-      <c r="X32" s="13">
+      <c r="X32" s="6">
         <v>0.6</v>
       </c>
-      <c r="Y32" s="13"/>
-      <c r="Z32" s="13"/>
-      <c r="AA32" s="13" t="s">
+      <c r="Y32" s="6"/>
+      <c r="Z32" s="6"/>
+      <c r="AA32" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="AB32" s="13"/>
-      <c r="AC32" s="13"/>
-      <c r="AD32" s="13">
+      <c r="AB32" s="6"/>
+      <c r="AC32" s="6"/>
+      <c r="AD32" s="6">
         <v>0.75</v>
       </c>
-      <c r="AE32" s="13"/>
-      <c r="AF32" s="13"/>
-      <c r="AG32" s="13">
+      <c r="AE32" s="6"/>
+      <c r="AF32" s="6"/>
+      <c r="AG32" s="6">
         <v>0.75</v>
       </c>
-      <c r="AH32" s="13"/>
-      <c r="AI32" s="17"/>
+      <c r="AH32" s="6"/>
+      <c r="AI32" s="7"/>
     </row>
     <row r="33" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A33" s="14" t="s">
+      <c r="A33" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="B33" s="13" t="s">
+      <c r="B33" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G33" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H33" s="13">
-        <v>1</v>
-      </c>
-      <c r="I33" s="13" t="s">
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H33" s="6">
+        <v>1</v>
+      </c>
+      <c r="I33" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="J33" s="13">
+      <c r="J33" s="6">
         <v>0.01</v>
       </c>
-      <c r="K33" s="13">
+      <c r="K33" s="6">
         <v>0.01</v>
       </c>
-      <c r="L33" s="13">
+      <c r="L33" s="6">
         <v>0.03</v>
       </c>
-      <c r="M33" s="13"/>
-      <c r="N33" s="13"/>
-      <c r="O33" s="13"/>
-      <c r="P33" s="13"/>
-      <c r="Q33" s="13"/>
-      <c r="R33" s="13"/>
-      <c r="S33" s="13">
+      <c r="M33" s="6"/>
+      <c r="N33" s="6"/>
+      <c r="O33" s="6"/>
+      <c r="P33" s="6"/>
+      <c r="Q33" s="6"/>
+      <c r="R33" s="6"/>
+      <c r="S33" s="6">
         <v>10</v>
       </c>
-      <c r="T33" s="13"/>
-      <c r="U33" s="13"/>
-      <c r="V33" s="13">
-        <v>0</v>
-      </c>
-      <c r="W33" s="13">
+      <c r="T33" s="6"/>
+      <c r="U33" s="6"/>
+      <c r="V33" s="6">
+        <v>0</v>
+      </c>
+      <c r="W33" s="6">
         <v>4</v>
       </c>
-      <c r="X33" s="13">
+      <c r="X33" s="6">
         <v>0.6</v>
       </c>
-      <c r="Y33" s="13"/>
-      <c r="Z33" s="13"/>
-      <c r="AA33" s="13" t="s">
+      <c r="Y33" s="6"/>
+      <c r="Z33" s="6"/>
+      <c r="AA33" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="AB33" s="13"/>
-      <c r="AC33" s="13"/>
-      <c r="AD33" s="13">
-        <v>1</v>
-      </c>
-      <c r="AE33" s="13"/>
-      <c r="AF33" s="13"/>
-      <c r="AG33" s="13">
-        <v>1</v>
-      </c>
-      <c r="AH33" s="13"/>
-      <c r="AI33" s="17"/>
+      <c r="AB33" s="6"/>
+      <c r="AC33" s="6"/>
+      <c r="AD33" s="6">
+        <v>1</v>
+      </c>
+      <c r="AE33" s="6"/>
+      <c r="AF33" s="6"/>
+      <c r="AG33" s="6">
+        <v>1</v>
+      </c>
+      <c r="AH33" s="6"/>
+      <c r="AI33" s="7"/>
     </row>
     <row r="34" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A34" s="14" t="s">
+      <c r="A34" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B34" s="13" t="s">
+      <c r="B34" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G34" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H34" s="13">
-        <v>1</v>
-      </c>
-      <c r="I34" s="13" t="s">
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34" s="6">
+        <v>1</v>
+      </c>
+      <c r="I34" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="J34" s="13">
+      <c r="J34" s="6">
         <v>0.01</v>
       </c>
-      <c r="K34" s="13">
+      <c r="K34" s="6">
         <v>0.01</v>
       </c>
-      <c r="L34" s="13">
+      <c r="L34" s="6">
         <v>0.03</v>
       </c>
-      <c r="M34" s="13"/>
-      <c r="N34" s="13"/>
-      <c r="O34" s="13"/>
-      <c r="P34" s="13"/>
-      <c r="Q34" s="13"/>
-      <c r="R34" s="13"/>
-      <c r="S34" s="13">
+      <c r="M34" s="6"/>
+      <c r="N34" s="6"/>
+      <c r="O34" s="6"/>
+      <c r="P34" s="6"/>
+      <c r="Q34" s="6"/>
+      <c r="R34" s="6"/>
+      <c r="S34" s="6">
         <v>10</v>
       </c>
-      <c r="T34" s="13"/>
-      <c r="U34" s="13"/>
-      <c r="V34" s="13">
-        <v>0</v>
-      </c>
-      <c r="W34" s="13">
+      <c r="T34" s="6"/>
+      <c r="U34" s="6"/>
+      <c r="V34" s="6">
+        <v>0</v>
+      </c>
+      <c r="W34" s="6">
         <v>4</v>
       </c>
-      <c r="X34" s="13">
+      <c r="X34" s="6">
         <v>0.6</v>
       </c>
-      <c r="Y34" s="13"/>
-      <c r="Z34" s="13"/>
-      <c r="AA34" s="13" t="s">
+      <c r="Y34" s="6"/>
+      <c r="Z34" s="6"/>
+      <c r="AA34" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="AB34" s="13"/>
-      <c r="AC34" s="13"/>
-      <c r="AD34" s="13">
-        <v>1</v>
-      </c>
-      <c r="AE34" s="13"/>
-      <c r="AF34" s="13"/>
-      <c r="AG34" s="13">
-        <v>1</v>
-      </c>
-      <c r="AH34" s="13"/>
-      <c r="AI34" s="17"/>
+      <c r="AB34" s="6"/>
+      <c r="AC34" s="6"/>
+      <c r="AD34" s="6">
+        <v>1</v>
+      </c>
+      <c r="AE34" s="6"/>
+      <c r="AF34" s="6"/>
+      <c r="AG34" s="6">
+        <v>1</v>
+      </c>
+      <c r="AH34" s="6"/>
+      <c r="AI34" s="7"/>
     </row>
     <row r="35" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A35" s="14" t="s">
+      <c r="A35" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="B35" s="13" t="s">
+      <c r="B35" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13">
+      <c r="C35" s="6"/>
+      <c r="D35" s="6">
         <v>0.04</v>
       </c>
-      <c r="E35" s="13">
+      <c r="E35" s="6">
         <v>0.02</v>
       </c>
-      <c r="F35" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G35" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H35" s="13">
-        <v>1</v>
-      </c>
-      <c r="I35" s="13" t="s">
+      <c r="F35" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H35" s="6">
+        <v>1</v>
+      </c>
+      <c r="I35" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="J35" s="13">
+      <c r="J35" s="6">
         <v>0.02</v>
       </c>
-      <c r="K35" s="13">
+      <c r="K35" s="6">
         <v>0.09</v>
       </c>
-      <c r="L35" s="13">
+      <c r="L35" s="6">
         <v>0.04</v>
       </c>
-      <c r="M35" s="13"/>
-      <c r="N35" s="13"/>
-      <c r="O35" s="13"/>
-      <c r="P35" s="13"/>
-      <c r="Q35" s="13"/>
-      <c r="R35" s="13"/>
-      <c r="S35" s="13">
+      <c r="M35" s="6"/>
+      <c r="N35" s="6"/>
+      <c r="O35" s="6"/>
+      <c r="P35" s="6"/>
+      <c r="Q35" s="6"/>
+      <c r="R35" s="6"/>
+      <c r="S35" s="6">
         <v>10</v>
       </c>
-      <c r="T35" s="13"/>
-      <c r="U35" s="13"/>
-      <c r="V35" s="13">
-        <v>0</v>
-      </c>
-      <c r="W35" s="13">
+      <c r="T35" s="6"/>
+      <c r="U35" s="6"/>
+      <c r="V35" s="6">
+        <v>0</v>
+      </c>
+      <c r="W35" s="6">
         <v>6</v>
       </c>
-      <c r="X35" s="13">
+      <c r="X35" s="6">
         <v>0.6</v>
       </c>
-      <c r="Y35" s="13"/>
-      <c r="Z35" s="13"/>
-      <c r="AA35" s="13" t="s">
+      <c r="Y35" s="6"/>
+      <c r="Z35" s="6"/>
+      <c r="AA35" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="AB35" s="13"/>
-      <c r="AC35" s="13"/>
-      <c r="AD35" s="13">
-        <v>1</v>
-      </c>
-      <c r="AE35" s="13"/>
-      <c r="AF35" s="13"/>
-      <c r="AG35" s="13">
-        <v>1</v>
-      </c>
-      <c r="AH35" s="13"/>
-      <c r="AI35" s="17"/>
+      <c r="AB35" s="6"/>
+      <c r="AC35" s="6"/>
+      <c r="AD35" s="6">
+        <v>1</v>
+      </c>
+      <c r="AE35" s="6"/>
+      <c r="AF35" s="6"/>
+      <c r="AG35" s="6">
+        <v>1</v>
+      </c>
+      <c r="AH35" s="6"/>
+      <c r="AI35" s="7"/>
     </row>
     <row r="36" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A36" s="14" t="s">
+      <c r="A36" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B36" s="13" t="s">
+      <c r="B36" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13">
+      <c r="C36" s="6"/>
+      <c r="D36" s="6">
         <v>0.02</v>
       </c>
-      <c r="E36" s="13">
+      <c r="E36" s="6">
         <v>0.03</v>
       </c>
-      <c r="F36" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="G36" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H36" s="13">
-        <v>1</v>
-      </c>
-      <c r="I36" s="13" t="s">
+      <c r="F36" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H36" s="6">
+        <v>1</v>
+      </c>
+      <c r="I36" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="J36" s="13">
+      <c r="J36" s="6">
         <v>0.02</v>
       </c>
-      <c r="K36" s="13">
+      <c r="K36" s="6">
         <v>0.03</v>
       </c>
-      <c r="L36" s="13">
+      <c r="L36" s="6">
         <v>0.08</v>
       </c>
-      <c r="M36" s="13"/>
-      <c r="N36" s="13"/>
-      <c r="O36" s="13"/>
-      <c r="P36" s="13"/>
-      <c r="Q36" s="13"/>
-      <c r="R36" s="13"/>
-      <c r="S36" s="13">
+      <c r="M36" s="6"/>
+      <c r="N36" s="6"/>
+      <c r="O36" s="6"/>
+      <c r="P36" s="6"/>
+      <c r="Q36" s="6"/>
+      <c r="R36" s="6"/>
+      <c r="S36" s="6">
         <v>5</v>
       </c>
-      <c r="T36" s="13"/>
-      <c r="U36" s="13"/>
-      <c r="V36" s="13">
-        <v>0</v>
-      </c>
-      <c r="W36" s="13">
+      <c r="T36" s="6"/>
+      <c r="U36" s="6"/>
+      <c r="V36" s="6">
+        <v>0</v>
+      </c>
+      <c r="W36" s="6">
         <v>6</v>
       </c>
-      <c r="X36" s="13">
+      <c r="X36" s="6">
         <v>0.6</v>
       </c>
-      <c r="Y36" s="13"/>
-      <c r="Z36" s="13"/>
-      <c r="AA36" s="13" t="s">
+      <c r="Y36" s="6"/>
+      <c r="Z36" s="6"/>
+      <c r="AA36" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="AB36" s="13"/>
-      <c r="AC36" s="13"/>
-      <c r="AD36" s="13">
+      <c r="AB36" s="6"/>
+      <c r="AC36" s="6"/>
+      <c r="AD36" s="6">
         <v>0.75</v>
       </c>
-      <c r="AE36" s="13"/>
-      <c r="AF36" s="13"/>
-      <c r="AG36" s="13">
+      <c r="AE36" s="6"/>
+      <c r="AF36" s="6"/>
+      <c r="AG36" s="6">
         <v>0.75</v>
       </c>
-      <c r="AH36" s="13"/>
-      <c r="AI36" s="17"/>
+      <c r="AH36" s="6"/>
+      <c r="AI36" s="7"/>
     </row>
     <row r="37" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A37" s="15" t="s">
+      <c r="A37" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B37" s="16" t="s">
+      <c r="B37" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C37" s="16"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="G37" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="H37" s="16">
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H37" s="2">
         <v>2</v>
       </c>
-      <c r="I37" s="16" t="s">
+      <c r="I37" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="J37" s="16"/>
-      <c r="K37" s="16"/>
-      <c r="L37" s="16"/>
-      <c r="M37" s="16">
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2">
         <v>0.01</v>
       </c>
-      <c r="N37" s="16">
+      <c r="N37" s="2">
         <v>0.04</v>
       </c>
-      <c r="O37" s="16">
-        <v>0</v>
-      </c>
-      <c r="P37" s="16">
-        <v>0</v>
-      </c>
-      <c r="Q37" s="16">
+      <c r="O37" s="2">
+        <v>0</v>
+      </c>
+      <c r="P37" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="2">
         <v>0.01</v>
       </c>
-      <c r="R37" s="16">
+      <c r="R37" s="2">
         <v>0.03</v>
       </c>
-      <c r="S37" s="16"/>
-      <c r="T37" s="16">
+      <c r="S37" s="2"/>
+      <c r="T37" s="2">
         <v>50</v>
       </c>
-      <c r="U37" s="16">
+      <c r="U37" s="2">
         <v>50</v>
       </c>
-      <c r="V37" s="16">
-        <v>0</v>
-      </c>
-      <c r="W37" s="16">
+      <c r="V37" s="2">
+        <v>0</v>
+      </c>
+      <c r="W37" s="2">
         <v>3</v>
       </c>
-      <c r="X37" s="16"/>
-      <c r="Y37" s="16">
-        <v>1</v>
-      </c>
-      <c r="Z37" s="16">
+      <c r="X37" s="2"/>
+      <c r="Y37" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z37" s="2">
         <v>0.52</v>
       </c>
-      <c r="AA37" s="16" t="s">
+      <c r="AA37" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AB37" s="16"/>
-      <c r="AC37" s="16"/>
-      <c r="AD37" s="16"/>
-      <c r="AE37" s="16">
-        <v>0.5</v>
-      </c>
-      <c r="AF37" s="16">
-        <v>1</v>
-      </c>
-      <c r="AG37" s="16"/>
-      <c r="AH37" s="16">
-        <v>0.5</v>
-      </c>
-      <c r="AI37" s="18">
+      <c r="AB37" s="2"/>
+      <c r="AC37" s="2"/>
+      <c r="AD37" s="2"/>
+      <c r="AE37" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="AF37" s="2">
+        <v>1</v>
+      </c>
+      <c r="AG37" s="2"/>
+      <c r="AH37" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="AI37" s="3">
         <v>1</v>
       </c>
     </row>
@@ -5243,10 +5243,10 @@
         <v>0.01</v>
       </c>
       <c r="K43">
-        <v>0.08</v>
+        <v>0.15</v>
       </c>
       <c r="L43">
-        <v>0.09</v>
+        <v>0.19</v>
       </c>
       <c r="S43">
         <v>0.5</v>
@@ -5260,8 +5260,8 @@
       <c r="X43">
         <v>0.5</v>
       </c>
-      <c r="AA43" s="19" t="s">
-        <v>25</v>
+      <c r="AA43" s="14" t="s">
+        <v>113</v>
       </c>
       <c r="AD43">
         <v>0.995</v>
@@ -5293,10 +5293,10 @@
         <v>0.01</v>
       </c>
       <c r="K44">
-        <v>0.08</v>
+        <v>0.15</v>
       </c>
       <c r="L44">
-        <v>0.09</v>
+        <v>0.19</v>
       </c>
       <c r="S44">
         <v>0.5</v>
@@ -5310,8 +5310,8 @@
       <c r="X44">
         <v>0.5</v>
       </c>
-      <c r="AA44" s="19" t="s">
-        <v>25</v>
+      <c r="AA44" s="14" t="s">
+        <v>113</v>
       </c>
       <c r="AD44">
         <v>0.995</v>
@@ -5343,7 +5343,7 @@
         <v>0.01</v>
       </c>
       <c r="K45">
-        <v>0.08</v>
+        <v>0.15</v>
       </c>
       <c r="L45">
         <v>0.14000000000000001</v>
@@ -5360,8 +5360,8 @@
       <c r="X45">
         <v>0.5</v>
       </c>
-      <c r="AA45" s="19" t="s">
-        <v>25</v>
+      <c r="AA45" s="14" t="s">
+        <v>113</v>
       </c>
       <c r="AD45">
         <v>0.996</v>
@@ -5393,7 +5393,7 @@
         <v>0.01</v>
       </c>
       <c r="K46">
-        <v>0.08</v>
+        <v>0.15</v>
       </c>
       <c r="L46">
         <v>0.14000000000000001</v>
@@ -5410,8 +5410,8 @@
       <c r="X46">
         <v>0.5</v>
       </c>
-      <c r="AA46" s="19" t="s">
-        <v>25</v>
+      <c r="AA46" s="14" t="s">
+        <v>113</v>
       </c>
       <c r="AD46">
         <v>0.996</v>
@@ -5443,10 +5443,10 @@
         <v>0.01</v>
       </c>
       <c r="K47">
+        <v>0.17</v>
+      </c>
+      <c r="L47">
         <v>0.08</v>
-      </c>
-      <c r="L47">
-        <v>0.14000000000000001</v>
       </c>
       <c r="S47">
         <v>0.06</v>
@@ -5460,8 +5460,8 @@
       <c r="X47">
         <v>0.5</v>
       </c>
-      <c r="AA47" s="19" t="s">
-        <v>25</v>
+      <c r="AA47" s="14" t="s">
+        <v>113</v>
       </c>
       <c r="AD47">
         <v>0.997</v>
@@ -5493,10 +5493,10 @@
         <v>0.01</v>
       </c>
       <c r="K48">
+        <v>0.17</v>
+      </c>
+      <c r="L48">
         <v>0.08</v>
-      </c>
-      <c r="L48">
-        <v>0.14000000000000001</v>
       </c>
       <c r="S48">
         <v>0.06</v>
@@ -5510,8 +5510,8 @@
       <c r="X48">
         <v>0.5</v>
       </c>
-      <c r="AA48" s="19" t="s">
-        <v>25</v>
+      <c r="AA48" s="14" t="s">
+        <v>113</v>
       </c>
       <c r="AD48">
         <v>0.997</v>
@@ -5560,8 +5560,8 @@
       <c r="X49">
         <v>0.5</v>
       </c>
-      <c r="AA49" s="19" t="s">
-        <v>25</v>
+      <c r="AA49" s="14" t="s">
+        <v>113</v>
       </c>
       <c r="AD49">
         <v>0.995</v>
@@ -5610,8 +5610,8 @@
       <c r="X50">
         <v>0.5</v>
       </c>
-      <c r="AA50" s="19" t="s">
-        <v>25</v>
+      <c r="AA50" s="14" t="s">
+        <v>113</v>
       </c>
       <c r="AD50">
         <v>0.995</v>
@@ -5660,8 +5660,8 @@
       <c r="X51">
         <v>0.5</v>
       </c>
-      <c r="AA51" s="19" t="s">
-        <v>25</v>
+      <c r="AA51" s="14" t="s">
+        <v>113</v>
       </c>
       <c r="AD51">
         <v>0.996</v>
@@ -5710,8 +5710,8 @@
       <c r="X52">
         <v>0.5</v>
       </c>
-      <c r="AA52" s="19" t="s">
-        <v>25</v>
+      <c r="AA52" s="14" t="s">
+        <v>113</v>
       </c>
       <c r="AD52">
         <v>0.996</v>
@@ -5760,8 +5760,8 @@
       <c r="X53">
         <v>0.5</v>
       </c>
-      <c r="AA53" s="19" t="s">
-        <v>25</v>
+      <c r="AA53" s="14" t="s">
+        <v>113</v>
       </c>
       <c r="AD53">
         <v>0.997</v>
@@ -5810,8 +5810,8 @@
       <c r="X54">
         <v>0.5</v>
       </c>
-      <c r="AA54" s="19" t="s">
-        <v>25</v>
+      <c r="AA54" s="14" t="s">
+        <v>113</v>
       </c>
       <c r="AD54">
         <v>0.997</v>
@@ -5843,10 +5843,10 @@
         <v>0.01</v>
       </c>
       <c r="K55">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="L55">
-        <v>0.1</v>
+        <v>0.9</v>
       </c>
       <c r="S55">
         <v>0.5</v>
@@ -5860,8 +5860,8 @@
       <c r="X55">
         <v>0.5</v>
       </c>
-      <c r="AA55" s="19" t="s">
-        <v>25</v>
+      <c r="AA55" s="14" t="s">
+        <v>113</v>
       </c>
       <c r="AD55">
         <v>0.995</v>
@@ -5893,10 +5893,10 @@
         <v>0.01</v>
       </c>
       <c r="K56">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="L56">
-        <v>0.1</v>
+        <v>0.9</v>
       </c>
       <c r="S56">
         <v>0.5</v>
@@ -5910,8 +5910,8 @@
       <c r="X56">
         <v>0.5</v>
       </c>
-      <c r="AA56" s="19" t="s">
-        <v>25</v>
+      <c r="AA56" s="14" t="s">
+        <v>113</v>
       </c>
       <c r="AD56">
         <v>0.995</v>
@@ -5943,10 +5943,10 @@
         <v>0.01</v>
       </c>
       <c r="K57">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="L57">
-        <v>0.125</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="S57">
         <v>0.08</v>
@@ -5960,8 +5960,8 @@
       <c r="X57">
         <v>0.5</v>
       </c>
-      <c r="AA57" s="19" t="s">
-        <v>25</v>
+      <c r="AA57" s="14" t="s">
+        <v>113</v>
       </c>
       <c r="AD57">
         <v>0.996</v>
@@ -5993,10 +5993,10 @@
         <v>0.01</v>
       </c>
       <c r="K58">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="L58">
-        <v>0.125</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="S58">
         <v>0.08</v>
@@ -6010,8 +6010,8 @@
       <c r="X58">
         <v>0.5</v>
       </c>
-      <c r="AA58" s="19" t="s">
-        <v>25</v>
+      <c r="AA58" s="14" t="s">
+        <v>113</v>
       </c>
       <c r="AD58">
         <v>0.996</v>
@@ -6043,10 +6043,10 @@
         <v>0.01</v>
       </c>
       <c r="K59">
-        <v>0.15</v>
+        <v>0.22</v>
       </c>
       <c r="L59">
-        <v>0.125</v>
+        <v>0.17</v>
       </c>
       <c r="S59">
         <v>0.06</v>
@@ -6060,8 +6060,8 @@
       <c r="X59">
         <v>0.5</v>
       </c>
-      <c r="AA59" s="19" t="s">
-        <v>25</v>
+      <c r="AA59" s="14" t="s">
+        <v>113</v>
       </c>
       <c r="AD59">
         <v>0.997</v>
@@ -6093,10 +6093,10 @@
         <v>0.01</v>
       </c>
       <c r="K60">
-        <v>0.15</v>
+        <v>0.22</v>
       </c>
       <c r="L60">
-        <v>0.125</v>
+        <v>0.17</v>
       </c>
       <c r="S60">
         <v>0.06</v>
@@ -6110,8 +6110,8 @@
       <c r="X60">
         <v>0.5</v>
       </c>
-      <c r="AA60" s="19" t="s">
-        <v>25</v>
+      <c r="AA60" s="14" t="s">
+        <v>113</v>
       </c>
       <c r="AD60">
         <v>0.997</v>

</xml_diff>